<commit_message>
Esp. de Req., Trazabilidad, Herramientas
</commit_message>
<xml_diff>
--- a/Fases_de_desarrollo/01-Inicio/05- Gestion de Proyecto/Matriz de Trazabilidad.xlsx
+++ b/Fases_de_desarrollo/01-Inicio/05- Gestion de Proyecto/Matriz de Trazabilidad.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="45">
   <si>
     <t>RF01</t>
   </si>
@@ -122,15 +122,6 @@
   </si>
   <si>
     <t>RF23</t>
-  </si>
-  <si>
-    <t>RF24</t>
-  </si>
-  <si>
-    <t>RF25</t>
-  </si>
-  <si>
-    <t>RF26</t>
   </si>
   <si>
     <t>CU02 - Asignar Caso de Uso</t>
@@ -544,11 +535,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA22"/>
+  <dimension ref="A1:X22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AD19" sqref="AD19"/>
+      <selection pane="topRight" activeCell="AD16" sqref="AD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,7 +550,7 @@
     <col min="8" max="27" width="5.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -629,212 +620,203 @@
       <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" t="s">
+        <v>44</v>
+      </c>
+      <c r="N2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="P3" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="W4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F2" t="s">
-        <v>47</v>
-      </c>
-      <c r="J2" t="s">
-        <v>47</v>
-      </c>
-      <c r="N2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="R5" t="s">
+        <v>44</v>
+      </c>
+      <c r="S5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="P3" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="W4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="B8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I8" t="s">
+        <v>44</v>
+      </c>
+      <c r="R8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="R5" t="s">
-        <v>47</v>
-      </c>
-      <c r="S5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="T6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="C9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" t="s">
+        <v>44</v>
+      </c>
+      <c r="L9" t="s">
+        <v>44</v>
+      </c>
+      <c r="N9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I8" t="s">
-        <v>47</v>
-      </c>
-      <c r="R8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="O11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D9" t="s">
-        <v>47</v>
-      </c>
-      <c r="L9" t="s">
-        <v>47</v>
-      </c>
-      <c r="N9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="D12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" t="s">
+        <v>44</v>
+      </c>
+      <c r="N12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="O11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="N14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D12" t="s">
-        <v>47</v>
-      </c>
-      <c r="E12" t="s">
-        <v>47</v>
-      </c>
-      <c r="N12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="K15" t="s">
+        <v>44</v>
+      </c>
+      <c r="L15" t="s">
+        <v>44</v>
+      </c>
+      <c r="N15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="N14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K15" t="s">
-        <v>47</v>
-      </c>
-      <c r="L15" t="s">
-        <v>47</v>
-      </c>
-      <c r="N15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="M17" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="N17" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L18" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>